<commit_message>
Update compare results for public review
Added some comments and changed some colors so people can read my
results more easily.
</commit_message>
<xml_diff>
--- a/Logical-Analyzer-traces/decode-sequencenumber/decode-sequencenumber.xlsx
+++ b/Logical-Analyzer-traces/decode-sequencenumber/decode-sequencenumber.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="part1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,40 @@
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="L15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These values changed because I pressed the medium button instead of the full button. With other buttons I expect these 2 bytes to change.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,10 +97,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,10 +158,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -411,26 +467,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
@@ -454,10 +513,10 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
@@ -465,16 +524,16 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>170</v>
-      </c>
-      <c r="B2">
-        <v>170</v>
-      </c>
-      <c r="C2">
-        <v>170</v>
-      </c>
-      <c r="D2">
+      <c r="A2" s="3">
+        <v>170</v>
+      </c>
+      <c r="B2" s="3">
+        <v>170</v>
+      </c>
+      <c r="C2" s="3">
+        <v>170</v>
+      </c>
+      <c r="D2" s="3">
         <v>170</v>
       </c>
       <c r="E2">
@@ -509,16 +568,16 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>170</v>
-      </c>
-      <c r="B3">
-        <v>170</v>
-      </c>
-      <c r="C3">
-        <v>170</v>
-      </c>
-      <c r="D3">
+      <c r="A3" s="3">
+        <v>170</v>
+      </c>
+      <c r="B3" s="3">
+        <v>170</v>
+      </c>
+      <c r="C3" s="3">
+        <v>170</v>
+      </c>
+      <c r="D3" s="3">
         <v>170</v>
       </c>
       <c r="E3">
@@ -553,16 +612,16 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>170</v>
-      </c>
-      <c r="B4">
-        <v>170</v>
-      </c>
-      <c r="C4">
-        <v>170</v>
-      </c>
-      <c r="D4">
+      <c r="A4" s="3">
+        <v>170</v>
+      </c>
+      <c r="B4" s="3">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3">
+        <v>170</v>
+      </c>
+      <c r="D4" s="3">
         <v>170</v>
       </c>
       <c r="E4">
@@ -597,16 +656,16 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>173</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>173</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>173</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>173</v>
       </c>
       <c r="E5">
@@ -641,16 +700,16 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>51</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>51</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>51</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>51</v>
       </c>
       <c r="E6">
@@ -685,16 +744,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>83</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>83</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>83</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>83</v>
       </c>
       <c r="E7">
@@ -729,16 +788,16 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>74</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>74</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>74</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>74</v>
       </c>
       <c r="E8">
@@ -773,16 +832,16 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>203</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>203</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>203</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>203</v>
       </c>
       <c r="E9">
@@ -817,16 +876,16 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>76</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>76</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>76</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>76</v>
       </c>
       <c r="E10">
@@ -861,16 +920,16 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>205</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>205</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>205</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>205</v>
       </c>
       <c r="E11">
@@ -905,16 +964,16 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>84</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>84</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>84</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>84</v>
       </c>
       <c r="E12">
@@ -949,16 +1008,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>213</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>213</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>213</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>213</v>
       </c>
       <c r="E13">
@@ -993,16 +1052,16 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>85</v>
-      </c>
-      <c r="B14">
-        <v>85</v>
-      </c>
-      <c r="C14">
-        <v>85</v>
-      </c>
-      <c r="D14">
+      <c r="A14" s="3">
+        <v>85</v>
+      </c>
+      <c r="B14" s="3">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3">
         <v>85</v>
       </c>
       <c r="E14">
@@ -1037,16 +1096,16 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>51</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>51</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>51</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>51</v>
       </c>
       <c r="E15">
@@ -1081,16 +1140,16 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>82</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>82</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>82</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>82</v>
       </c>
       <c r="E16">
@@ -1125,16 +1184,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>180</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>180</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>180</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>180</v>
       </c>
       <c r="E17">
@@ -1169,16 +1228,16 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>170</v>
-      </c>
-      <c r="B18">
-        <v>170</v>
-      </c>
-      <c r="C18">
-        <v>170</v>
-      </c>
-      <c r="D18">
+      <c r="A18" s="3">
+        <v>170</v>
+      </c>
+      <c r="B18" s="3">
+        <v>170</v>
+      </c>
+      <c r="C18" s="3">
+        <v>170</v>
+      </c>
+      <c r="D18" s="3">
         <v>170</v>
       </c>
       <c r="E18">
@@ -1213,16 +1272,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>171</v>
-      </c>
-      <c r="B19">
-        <v>171</v>
-      </c>
-      <c r="C19">
-        <v>171</v>
-      </c>
-      <c r="D19">
+      <c r="A19" s="3">
+        <v>171</v>
+      </c>
+      <c r="B19" s="3">
+        <v>171</v>
+      </c>
+      <c r="C19" s="3">
+        <v>171</v>
+      </c>
+      <c r="D19" s="3">
         <v>171</v>
       </c>
       <c r="E19">
@@ -1257,16 +1316,16 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>85</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="4">
+        <v>85</v>
+      </c>
+      <c r="B20" s="4">
         <v>77</v>
       </c>
-      <c r="C20" s="1">
-        <v>85</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="4">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4">
         <v>85</v>
       </c>
       <c r="E20" s="1">
@@ -1301,16 +1360,16 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>75</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="4">
         <v>77</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <v>75</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>85</v>
       </c>
       <c r="E21" s="1">
@@ -1344,124 +1403,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f t="shared" ref="A23:C23" si="0">DEC2BIN(A20)</f>
-        <v>1010101</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>1001101</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>1010101</v>
-      </c>
-      <c r="D23" t="str">
-        <f>DEC2BIN(D20)</f>
-        <v>1010101</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" ref="E23:N23" si="1">DEC2BIN(E20)</f>
-        <v>1010101</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="K23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" si="1"/>
-        <v>1010101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f t="shared" ref="A24:C24" si="2">DEC2BIN(A21)</f>
-        <v>1001011</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" si="2"/>
-        <v>1001101</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="2"/>
-        <v>1001011</v>
-      </c>
-      <c r="D24" t="str">
-        <f>DEC2BIN(D21)</f>
-        <v>1010101</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" ref="E24:N24" si="3">DEC2BIN(E21)</f>
-        <v>110101</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="3"/>
-        <v>110101</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" si="3"/>
-        <v>1001011</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" si="3"/>
-        <v>1001011</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1469,23 +1414,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
@@ -1509,10 +1457,10 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
@@ -1520,16 +1468,16 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>170</v>
-      </c>
-      <c r="B2">
-        <v>170</v>
-      </c>
-      <c r="C2">
-        <v>170</v>
-      </c>
-      <c r="D2">
+      <c r="A2" s="3">
+        <v>170</v>
+      </c>
+      <c r="B2" s="3">
+        <v>170</v>
+      </c>
+      <c r="C2" s="3">
+        <v>170</v>
+      </c>
+      <c r="D2" s="3">
         <v>170</v>
       </c>
       <c r="E2">
@@ -1564,16 +1512,16 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>170</v>
-      </c>
-      <c r="B3">
-        <v>170</v>
-      </c>
-      <c r="C3">
-        <v>170</v>
-      </c>
-      <c r="D3">
+      <c r="A3" s="3">
+        <v>170</v>
+      </c>
+      <c r="B3" s="3">
+        <v>170</v>
+      </c>
+      <c r="C3" s="3">
+        <v>170</v>
+      </c>
+      <c r="D3" s="3">
         <v>170</v>
       </c>
       <c r="E3">
@@ -1608,16 +1556,16 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>170</v>
-      </c>
-      <c r="B4">
-        <v>170</v>
-      </c>
-      <c r="C4">
-        <v>170</v>
-      </c>
-      <c r="D4">
+      <c r="A4" s="3">
+        <v>170</v>
+      </c>
+      <c r="B4" s="3">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3">
+        <v>170</v>
+      </c>
+      <c r="D4" s="3">
         <v>170</v>
       </c>
       <c r="E4">
@@ -1652,16 +1600,16 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>170</v>
-      </c>
-      <c r="B5">
-        <v>170</v>
-      </c>
-      <c r="C5">
-        <v>170</v>
-      </c>
-      <c r="D5">
+      <c r="A5" s="3">
+        <v>170</v>
+      </c>
+      <c r="B5" s="3">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3">
+        <v>170</v>
+      </c>
+      <c r="D5" s="3">
         <v>170</v>
       </c>
       <c r="E5">
@@ -1696,16 +1644,16 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>170</v>
-      </c>
-      <c r="B6">
-        <v>170</v>
-      </c>
-      <c r="C6">
-        <v>170</v>
-      </c>
-      <c r="D6">
+      <c r="A6" s="3">
+        <v>170</v>
+      </c>
+      <c r="B6" s="3">
+        <v>170</v>
+      </c>
+      <c r="C6" s="3">
+        <v>170</v>
+      </c>
+      <c r="D6" s="3">
         <v>170</v>
       </c>
       <c r="E6">
@@ -1740,16 +1688,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>170</v>
-      </c>
-      <c r="B7">
-        <v>170</v>
-      </c>
-      <c r="C7">
-        <v>170</v>
-      </c>
-      <c r="D7">
+      <c r="A7" s="3">
+        <v>170</v>
+      </c>
+      <c r="B7" s="3">
+        <v>170</v>
+      </c>
+      <c r="C7" s="3">
+        <v>170</v>
+      </c>
+      <c r="D7" s="3">
         <v>170</v>
       </c>
       <c r="E7">
@@ -1784,16 +1732,16 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>170</v>
-      </c>
-      <c r="B8">
-        <v>170</v>
-      </c>
-      <c r="C8">
-        <v>170</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="3">
+        <v>170</v>
+      </c>
+      <c r="B8" s="3">
+        <v>170</v>
+      </c>
+      <c r="C8" s="3">
+        <v>170</v>
+      </c>
+      <c r="D8" s="3">
         <v>170</v>
       </c>
       <c r="E8">
@@ -1828,16 +1776,16 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>171</v>
-      </c>
-      <c r="B9">
-        <v>171</v>
-      </c>
-      <c r="C9">
-        <v>171</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="3">
+        <v>171</v>
+      </c>
+      <c r="B9" s="3">
+        <v>171</v>
+      </c>
+      <c r="C9" s="3">
+        <v>171</v>
+      </c>
+      <c r="D9" s="3">
         <v>171</v>
       </c>
       <c r="E9">
@@ -1872,16 +1820,16 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>254</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>254</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>254</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>254</v>
       </c>
       <c r="E10">
@@ -1916,16 +1864,16 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11">
@@ -1960,16 +1908,16 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>179</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>179</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>179</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>179</v>
       </c>
       <c r="E12">
@@ -2004,16 +1952,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>42</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>42</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>42</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>42</v>
       </c>
       <c r="E13">
@@ -2048,16 +1996,16 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>171</v>
-      </c>
-      <c r="B14">
-        <v>171</v>
-      </c>
-      <c r="C14">
-        <v>171</v>
-      </c>
-      <c r="D14">
+      <c r="A14" s="3">
+        <v>171</v>
+      </c>
+      <c r="B14" s="3">
+        <v>171</v>
+      </c>
+      <c r="C14" s="3">
+        <v>171</v>
+      </c>
+      <c r="D14" s="3">
         <v>171</v>
       </c>
       <c r="E14">
@@ -2092,16 +2040,16 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>42</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>42</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>42</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>42</v>
       </c>
       <c r="E15">
@@ -2136,16 +2084,16 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>149</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>149</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>149</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>149</v>
       </c>
       <c r="E16">
@@ -2180,16 +2128,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>154</v>
-      </c>
-      <c r="B17">
-        <v>154</v>
-      </c>
-      <c r="C17">
-        <v>154</v>
-      </c>
-      <c r="D17">
+      <c r="A17" s="3">
+        <v>154</v>
+      </c>
+      <c r="B17" s="3">
+        <v>154</v>
+      </c>
+      <c r="C17" s="3">
+        <v>154</v>
+      </c>
+      <c r="D17" s="3">
         <v>154</v>
       </c>
       <c r="E17">
@@ -2224,16 +2172,16 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>102</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>102</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>102</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>102</v>
       </c>
       <c r="E18">
@@ -2268,16 +2216,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>89</v>
-      </c>
-      <c r="B19">
-        <v>89</v>
-      </c>
-      <c r="C19">
-        <v>89</v>
-      </c>
-      <c r="D19">
+      <c r="A19" s="3">
+        <v>89</v>
+      </c>
+      <c r="B19" s="3">
+        <v>89</v>
+      </c>
+      <c r="C19" s="3">
+        <v>89</v>
+      </c>
+      <c r="D19" s="3">
         <v>89</v>
       </c>
       <c r="E19">
@@ -2312,16 +2260,16 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>154</v>
-      </c>
-      <c r="B20">
-        <v>154</v>
-      </c>
-      <c r="C20">
-        <v>154</v>
-      </c>
-      <c r="D20">
+      <c r="A20" s="3">
+        <v>154</v>
+      </c>
+      <c r="B20" s="3">
+        <v>154</v>
+      </c>
+      <c r="C20" s="3">
+        <v>154</v>
+      </c>
+      <c r="D20" s="3">
         <v>154</v>
       </c>
       <c r="E20">
@@ -2356,16 +2304,16 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>165</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>165</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>165</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>165</v>
       </c>
       <c r="E21">
@@ -2400,16 +2348,16 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>169</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>169</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>169</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>169</v>
       </c>
       <c r="E22">
@@ -2444,16 +2392,16 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>169</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>169</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>169</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>169</v>
       </c>
       <c r="E23">
@@ -2488,16 +2436,16 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>154</v>
-      </c>
-      <c r="B24">
-        <v>154</v>
-      </c>
-      <c r="C24">
-        <v>154</v>
-      </c>
-      <c r="D24">
+      <c r="A24" s="3">
+        <v>154</v>
+      </c>
+      <c r="B24" s="3">
+        <v>154</v>
+      </c>
+      <c r="C24" s="3">
+        <v>154</v>
+      </c>
+      <c r="D24" s="3">
         <v>154</v>
       </c>
       <c r="E24">
@@ -2532,16 +2480,16 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>86</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>86</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>86</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>86</v>
       </c>
       <c r="E25">
@@ -2576,16 +2524,16 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>149</v>
       </c>
-      <c r="B26">
-        <v>89</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="3">
+        <v>89</v>
+      </c>
+      <c r="C26" s="3">
         <v>153</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>153</v>
       </c>
       <c r="E26">
@@ -2620,16 +2568,16 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="4">
         <v>165</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="4">
         <v>169</v>
       </c>
-      <c r="C27" s="1">
-        <v>154</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="4">
+        <v>154</v>
+      </c>
+      <c r="D27" s="4">
         <v>149</v>
       </c>
       <c r="E27" s="1">
@@ -2664,37 +2612,37 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="4">
         <v>166</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>102</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <v>102</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="4">
         <v>166</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>102</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>102</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>102</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>102</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="1">
         <v>102</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="1">
         <v>102</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="1">
         <v>102</v>
       </c>
       <c r="L28" s="1">
@@ -2708,16 +2656,16 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>89</v>
-      </c>
-      <c r="B29">
-        <v>89</v>
-      </c>
-      <c r="C29">
-        <v>89</v>
-      </c>
-      <c r="D29">
+      <c r="A29" s="3">
+        <v>89</v>
+      </c>
+      <c r="B29" s="3">
+        <v>89</v>
+      </c>
+      <c r="C29" s="3">
+        <v>89</v>
+      </c>
+      <c r="D29" s="3">
         <v>89</v>
       </c>
       <c r="E29">
@@ -2752,16 +2700,16 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>150</v>
-      </c>
-      <c r="B30">
-        <v>150</v>
-      </c>
-      <c r="C30">
-        <v>150</v>
-      </c>
-      <c r="D30">
+      <c r="A30" s="3">
+        <v>150</v>
+      </c>
+      <c r="B30" s="3">
+        <v>150</v>
+      </c>
+      <c r="C30" s="3">
+        <v>150</v>
+      </c>
+      <c r="D30" s="3">
         <v>150</v>
       </c>
       <c r="E30">
@@ -2796,16 +2744,16 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>170</v>
-      </c>
-      <c r="B31">
-        <v>170</v>
-      </c>
-      <c r="C31">
-        <v>170</v>
-      </c>
-      <c r="D31">
+      <c r="A31" s="3">
+        <v>170</v>
+      </c>
+      <c r="B31" s="3">
+        <v>170</v>
+      </c>
+      <c r="C31" s="3">
+        <v>170</v>
+      </c>
+      <c r="D31" s="3">
         <v>170</v>
       </c>
       <c r="E31">
@@ -2840,16 +2788,16 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>165</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>165</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>165</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="3">
         <v>165</v>
       </c>
       <c r="E32">
@@ -2884,16 +2832,16 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>101</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>101</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>101</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <v>101</v>
       </c>
       <c r="E33">
@@ -2928,16 +2876,16 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>90</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>90</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>90</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>90</v>
       </c>
       <c r="E34">
@@ -2972,16 +2920,16 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>150</v>
-      </c>
-      <c r="B35">
-        <v>150</v>
-      </c>
-      <c r="C35">
-        <v>150</v>
-      </c>
-      <c r="D35">
+      <c r="A35" s="3">
+        <v>150</v>
+      </c>
+      <c r="B35" s="3">
+        <v>150</v>
+      </c>
+      <c r="C35" s="3">
+        <v>150</v>
+      </c>
+      <c r="D35" s="3">
         <v>150</v>
       </c>
       <c r="E35">
@@ -3016,16 +2964,16 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>85</v>
-      </c>
-      <c r="B36">
-        <v>85</v>
-      </c>
-      <c r="C36">
-        <v>85</v>
-      </c>
-      <c r="D36">
+      <c r="A36" s="3">
+        <v>85</v>
+      </c>
+      <c r="B36" s="3">
+        <v>85</v>
+      </c>
+      <c r="C36" s="3">
+        <v>85</v>
+      </c>
+      <c r="D36" s="3">
         <v>85</v>
       </c>
       <c r="E36">
@@ -3060,16 +3008,16 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>149</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>149</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>149</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="3">
         <v>149</v>
       </c>
       <c r="E37">
@@ -3104,16 +3052,16 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>101</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>101</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>101</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="3">
         <v>101</v>
       </c>
       <c r="E38">
@@ -3148,16 +3096,16 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>89</v>
-      </c>
-      <c r="B39">
-        <v>89</v>
-      </c>
-      <c r="C39">
-        <v>89</v>
-      </c>
-      <c r="D39">
+      <c r="A39" s="3">
+        <v>89</v>
+      </c>
+      <c r="B39" s="3">
+        <v>89</v>
+      </c>
+      <c r="C39" s="3">
+        <v>89</v>
+      </c>
+      <c r="D39" s="3">
         <v>89</v>
       </c>
       <c r="E39">
@@ -3192,16 +3140,16 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>102</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>102</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>102</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="3">
         <v>102</v>
       </c>
       <c r="E40">
@@ -3236,16 +3184,16 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>85</v>
-      </c>
-      <c r="B41">
-        <v>85</v>
-      </c>
-      <c r="C41">
-        <v>85</v>
-      </c>
-      <c r="D41">
+      <c r="A41" s="3">
+        <v>85</v>
+      </c>
+      <c r="B41" s="3">
+        <v>85</v>
+      </c>
+      <c r="C41" s="3">
+        <v>85</v>
+      </c>
+      <c r="D41" s="3">
         <v>85</v>
       </c>
       <c r="E41">
@@ -3280,16 +3228,16 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>150</v>
-      </c>
-      <c r="B42">
-        <v>150</v>
-      </c>
-      <c r="C42">
-        <v>150</v>
-      </c>
-      <c r="D42">
+      <c r="A42" s="3">
+        <v>150</v>
+      </c>
+      <c r="B42" s="3">
+        <v>150</v>
+      </c>
+      <c r="C42" s="3">
+        <v>150</v>
+      </c>
+      <c r="D42" s="3">
         <v>150</v>
       </c>
       <c r="E42">
@@ -3324,16 +3272,16 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="4">
         <v>106</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="4">
         <v>105</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="4">
         <v>101</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="4">
         <v>106</v>
       </c>
       <c r="E43" s="1">
@@ -3368,16 +3316,16 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>170</v>
-      </c>
-      <c r="B44" s="1">
-        <v>170</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="A44" s="4">
+        <v>170</v>
+      </c>
+      <c r="B44" s="4">
+        <v>170</v>
+      </c>
+      <c r="C44" s="4">
         <v>169</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="4">
         <v>105</v>
       </c>
       <c r="E44" s="1">
@@ -3412,16 +3360,16 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="4">
         <v>106</v>
       </c>
-      <c r="B45" s="1">
-        <v>150</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="B45" s="4">
+        <v>150</v>
+      </c>
+      <c r="C45" s="4">
         <v>86</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="4">
         <v>170</v>
       </c>
       <c r="E45" s="1">
@@ -3456,16 +3404,16 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>172</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>172</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="3">
         <v>172</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="3">
         <v>172</v>
       </c>
       <c r="E46">
@@ -3500,16 +3448,16 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>170</v>
-      </c>
-      <c r="B47">
-        <v>170</v>
-      </c>
-      <c r="C47">
-        <v>170</v>
-      </c>
-      <c r="D47">
+      <c r="A47" s="3">
+        <v>170</v>
+      </c>
+      <c r="B47" s="3">
+        <v>170</v>
+      </c>
+      <c r="C47" s="3">
+        <v>170</v>
+      </c>
+      <c r="D47" s="3">
         <v>170</v>
       </c>
       <c r="E47">
@@ -3544,16 +3492,16 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>170</v>
-      </c>
-      <c r="B48">
-        <v>170</v>
-      </c>
-      <c r="C48">
-        <v>170</v>
-      </c>
-      <c r="D48">
+      <c r="A48" s="3">
+        <v>170</v>
+      </c>
+      <c r="B48" s="3">
+        <v>170</v>
+      </c>
+      <c r="C48" s="3">
+        <v>170</v>
+      </c>
+      <c r="D48" s="3">
         <v>170</v>
       </c>
       <c r="E48">
@@ -3588,16 +3536,16 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>170</v>
-      </c>
-      <c r="B49">
-        <v>170</v>
-      </c>
-      <c r="C49">
-        <v>170</v>
-      </c>
-      <c r="D49">
+      <c r="A49" s="3">
+        <v>170</v>
+      </c>
+      <c r="B49" s="3">
+        <v>170</v>
+      </c>
+      <c r="C49" s="3">
+        <v>170</v>
+      </c>
+      <c r="D49" s="3">
         <v>170</v>
       </c>
       <c r="E49">
@@ -3632,16 +3580,16 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>170</v>
-      </c>
-      <c r="B50">
-        <v>170</v>
-      </c>
-      <c r="C50">
-        <v>170</v>
-      </c>
-      <c r="D50">
+      <c r="A50" s="3">
+        <v>170</v>
+      </c>
+      <c r="B50" s="3">
+        <v>170</v>
+      </c>
+      <c r="C50" s="3">
+        <v>170</v>
+      </c>
+      <c r="D50" s="3">
         <v>170</v>
       </c>
       <c r="E50">
@@ -3676,16 +3624,16 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>170</v>
-      </c>
-      <c r="B51">
-        <v>170</v>
-      </c>
-      <c r="C51">
-        <v>170</v>
-      </c>
-      <c r="D51">
+      <c r="A51" s="3">
+        <v>170</v>
+      </c>
+      <c r="B51" s="3">
+        <v>170</v>
+      </c>
+      <c r="C51" s="3">
+        <v>170</v>
+      </c>
+      <c r="D51" s="3">
         <v>170</v>
       </c>
       <c r="E51">

</xml_diff>